<commit_message>
Massive rewrite. New access using properties.
</commit_message>
<xml_diff>
--- a/pyspreadsheet_test.xlsx
+++ b/pyspreadsheet_test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SheetA" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="SheetQuery" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Inventory" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Named Cells" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Type</t>
+    <t xml:space="preserve">Instrument</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -480,14 +480,14 @@
   </sheetPr>
   <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.87109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.5"/>
@@ -802,17 +802,17 @@
   </sheetPr>
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.37890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="9.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="7.87"/>
   </cols>
   <sheetData>
@@ -982,7 +982,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">

</xml_diff>

<commit_message>
Bugfix empty cells. New: text_not_empty
</commit_message>
<xml_diff>
--- a/pyspreadsheet_test.xlsx
+++ b/pyspreadsheet_test.xlsx
@@ -803,7 +803,7 @@
   <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.37890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -812,7 +812,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="19.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="7.87"/>
   </cols>
   <sheetData>
@@ -836,7 +836,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -848,9 +848,6 @@
       </c>
       <c r="E3" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="F3" s="10" t="n">
-        <v>1245678</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,7 +979,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.59375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">

</xml_diff>